<commit_message>
Updated switch & battery holder footprint, adjusted manual BOM
</commit_message>
<xml_diff>
--- a/ET-Abschlussgadget_2023/Materialliste.xlsx
+++ b/ET-Abschlussgadget_2023/Materialliste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FrosterOTG\Documents\ET-Abschlussgadget\ET-Abschlussgadget_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00347EB8-5C2D-4AA7-8345-BD9BCA7511D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E991F7D8-8376-424C-91D6-EF9B08327CFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="490" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,9 +42,6 @@
     <t>CR2032 Battery holder</t>
   </si>
   <si>
-    <t>https://www.lcsc.com/product-detail/span-style-background-color-ff0-Battery-span-Connectors_MYOUNG-MY-2032-22_C2902339.html</t>
-  </si>
-  <si>
     <t>IR LED</t>
   </si>
   <si>
@@ -60,9 +57,6 @@
     <t>Switch</t>
   </si>
   <si>
-    <t>https://www.lcsc.com/product-detail/span-style-background-color-ff0-Slide-span-Switches_SHOU-HAN-MSK-03-HB-125_C2858294.html</t>
-  </si>
-  <si>
     <t>110uF Cap</t>
   </si>
   <si>
@@ -73,6 +67,12 @@
   </si>
   <si>
     <t>https://www.lcsc.com/product-detail/Chip-Resistor-Surface-Mount_VO-SCR0805F590R_C3016757.html</t>
+  </si>
+  <si>
+    <t>https://www.lcsc.com/product-detail/span-style-background-color-ff0-Slide-span-Switches_SHOU-HAN-MSK12CO2-SZ_C2681568.html</t>
+  </si>
+  <si>
+    <t>https://www.lcsc.com/product-detail/span-style-background-color-ff0-Battery-span-Connectors_Q-J-C70373_C70373.html</t>
   </si>
 </sst>
 </file>
@@ -413,7 +413,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -442,55 +442,56 @@
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
+      <c r="B3" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
         <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
         <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1" xr:uid="{62E6A843-0099-46D2-99FA-985E4079E4D3}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{4BCD627E-5F2C-4AC5-B646-F72484BE5839}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Generated Output-Files, Added LCSC-Partnumbers to schematic
</commit_message>
<xml_diff>
--- a/ET-Abschlussgadget_2023/Materialliste.xlsx
+++ b/ET-Abschlussgadget_2023/Materialliste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FrosterOTG\Documents\ET-Abschlussgadget\ET-Abschlussgadget_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E991F7D8-8376-424C-91D6-EF9B08327CFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F841D7-76BA-4942-BF4A-9CAF799DE767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="490" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,13 +66,13 @@
     <t>590 Ohm Resistor</t>
   </si>
   <si>
-    <t>https://www.lcsc.com/product-detail/Chip-Resistor-Surface-Mount_VO-SCR0805F590R_C3016757.html</t>
-  </si>
-  <si>
     <t>https://www.lcsc.com/product-detail/span-style-background-color-ff0-Slide-span-Switches_SHOU-HAN-MSK12CO2-SZ_C2681568.html</t>
   </si>
   <si>
     <t>https://www.lcsc.com/product-detail/span-style-background-color-ff0-Battery-span-Connectors_Q-J-C70373_C70373.html</t>
+  </si>
+  <si>
+    <t>https://www.lcsc.com/product-detail/Chip-span-style-background-color-ff0-Resistor-span-Surface-Mount_Sunway-SC0603J5600F2BNRH_C5140946.html</t>
   </si>
 </sst>
 </file>
@@ -413,7 +413,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -443,14 +443,14 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -467,7 +467,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -482,16 +482,18 @@
       <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="B8" t="s">
-        <v>13</v>
+      <c r="B8" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1" xr:uid="{62E6A843-0099-46D2-99FA-985E4079E4D3}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{4BCD627E-5F2C-4AC5-B646-F72484BE5839}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{02991F0F-D553-48B2-8B51-4A5936166B41}"/>
+    <hyperlink ref="B8" r:id="rId4" xr:uid="{2294E385-21E0-4278-B4D0-3C4241E876DA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Replaced all footprints exept 0603-resistor with LCSC-footprints, generated new production-files, replaced 0805-cap with 0603-cap inside materialliste
</commit_message>
<xml_diff>
--- a/ET-Abschlussgadget_2023/Materialliste.xlsx
+++ b/ET-Abschlussgadget_2023/Materialliste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FrosterOTG\Documents\ET-Abschlussgadget\ET-Abschlussgadget_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38D1D95B-02B0-4102-8B09-1A5AC521639F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91BC4064-8AD3-4E29-8D99-467DF05DA0B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="490" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -60,9 +60,6 @@
     <t>110uF Cap</t>
   </si>
   <si>
-    <t>https://www.lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_FH-Guangdong-Fenghua-Advanced-Tech-0805B104K500NT_C38141.html</t>
-  </si>
-  <si>
     <t>590 Ohm Resistor</t>
   </si>
   <si>
@@ -73,6 +70,9 @@
   </si>
   <si>
     <t>https://www.lcsc.com/product-detail/Chip-span-style-background-color-ff0-Resistor-span-Surface-Mount_Sunway-SC0603J5600F2BNRH_C5140946.html</t>
+  </si>
+  <si>
+    <t>https://www.lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_CCTC-TCC0603X7R104K500CT_C282519.html</t>
   </si>
 </sst>
 </file>
@@ -413,7 +413,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -434,7 +434,7 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -443,7 +443,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -467,7 +467,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -475,15 +475,15 @@
         <v>10</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -494,8 +494,9 @@
     <hyperlink ref="B8" r:id="rId4" xr:uid="{2294E385-21E0-4278-B4D0-3C4241E876DA}"/>
     <hyperlink ref="B7" r:id="rId5" xr:uid="{10ED20AD-63CB-4C58-AE96-E8B7AF100A9D}"/>
     <hyperlink ref="B5" r:id="rId6" xr:uid="{24E521FF-3E1D-4D3C-9FBF-EAF25DCE0821}"/>
+    <hyperlink ref="B2" r:id="rId7" xr:uid="{E52057A6-738E-4CAF-A90D-070530903F63}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId7"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Replaced parts in materialliste, replaced some footprints, generade production-files with JLC-plugin
</commit_message>
<xml_diff>
--- a/ET-Abschlussgadget_2023/Materialliste.xlsx
+++ b/ET-Abschlussgadget_2023/Materialliste.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FrosterOTG\Documents\ET-Abschlussgadget\ET-Abschlussgadget_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91BC4064-8AD3-4E29-8D99-467DF05DA0B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43111B06-CCEB-4348-9BEB-551824833AB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="490" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
   <si>
     <t>Typ</t>
   </si>
@@ -57,12 +57,6 @@
     <t>Switch</t>
   </si>
   <si>
-    <t>110uF Cap</t>
-  </si>
-  <si>
-    <t>590 Ohm Resistor</t>
-  </si>
-  <si>
     <t>https://www.lcsc.com/product-detail/span-style-background-color-ff0-Slide-span-Switches_SHOU-HAN-MSK12CO2-SZ_C2681568.html</t>
   </si>
   <si>
@@ -73,6 +67,33 @@
   </si>
   <si>
     <t>https://www.lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_CCTC-TCC0603X7R104K500CT_C282519.html</t>
+  </si>
+  <si>
+    <t>560 Ohm Resistor</t>
+  </si>
+  <si>
+    <t>NEW</t>
+  </si>
+  <si>
+    <t>https://www.lcsc.com/product-detail/Infrared-IR-LEDs_XSSY-XS-IR04A05-802_C5205266.html</t>
+  </si>
+  <si>
+    <t>100nF Cap</t>
+  </si>
+  <si>
+    <t>https://www.lcsc.com/product-detail/Chip-Resistor-Surface-Mount_UNI-ROYAL-Uniroyal-Elec-0603WAJ0561T5E_C25247.html</t>
+  </si>
+  <si>
+    <t>N-MOSFET</t>
+  </si>
+  <si>
+    <t>https://www.lcsc.com/product-detail/MOSFETs_YONGYUTAI-SI2302_C2891732.html</t>
+  </si>
+  <si>
+    <t>1M Ohm Resistor</t>
+  </si>
+  <si>
+    <t>https://www.lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Sunway-SC0603F1004F2BNRH_C3152128.html</t>
   </si>
 </sst>
 </file>
@@ -410,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -443,7 +464,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -467,23 +488,100 @@
         <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="2" t="s">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>14</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -495,8 +593,15 @@
     <hyperlink ref="B7" r:id="rId5" xr:uid="{10ED20AD-63CB-4C58-AE96-E8B7AF100A9D}"/>
     <hyperlink ref="B5" r:id="rId6" xr:uid="{24E521FF-3E1D-4D3C-9FBF-EAF25DCE0821}"/>
     <hyperlink ref="B2" r:id="rId7" xr:uid="{E52057A6-738E-4CAF-A90D-070530903F63}"/>
+    <hyperlink ref="B15" r:id="rId8" xr:uid="{B24EB826-F512-433C-B7BE-1F0D833C963F}"/>
+    <hyperlink ref="B12" r:id="rId9" xr:uid="{5EE834CF-F82A-4546-A6A7-3B79699D1662}"/>
+    <hyperlink ref="B13" r:id="rId10" xr:uid="{5C84561E-2099-485E-AF08-974B31BC4BB6}"/>
+    <hyperlink ref="B17" r:id="rId11" xr:uid="{AC080943-B203-4C6F-9DAD-4D553E4009EF}"/>
+    <hyperlink ref="B16" r:id="rId12" xr:uid="{516050F3-164C-420F-9EA6-29A635A19A76}"/>
+    <hyperlink ref="B14" r:id="rId13" xr:uid="{B722BA65-DEFE-43AE-9FD1-FB515C14F961}"/>
+    <hyperlink ref="B11" r:id="rId14" xr:uid="{630E15A2-6CF7-4F14-8DD1-20F350C7E2AB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId8"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>